<commit_message>
My biggest commit yet
</commit_message>
<xml_diff>
--- a/Tests for our CPU.xlsx
+++ b/Tests for our CPU.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\GitHub\IAC-Coursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABE1871-A85D-4A8B-A6A6-8D9B110AF1AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1B04E8-2AAB-4FD6-B3AD-0BD6C75E02F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test 1" sheetId="1" r:id="rId1"/>
     <sheet name="Test2" sheetId="2" r:id="rId2"/>
     <sheet name="Test 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Test 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Test 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Test 6" sheetId="7" r:id="rId6"/>
+    <sheet name="Test 7" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="130">
   <si>
     <t>mem[0x0010] = 0x0000FF00</t>
   </si>
@@ -180,13 +184,250 @@
   </si>
   <si>
     <t>$v0 = 0x00000004</t>
+  </si>
+  <si>
+    <t>$t1 = 0xBFC00000</t>
+  </si>
+  <si>
+    <t>$t1 = 0xBFC00014</t>
+  </si>
+  <si>
+    <t>SKIPPED</t>
+  </si>
+  <si>
+    <t>$v0 = 0x00000024</t>
+  </si>
+  <si>
+    <t>$v0 = 0x00000028</t>
+  </si>
+  <si>
+    <t>$t0 = 0xBFC00028</t>
+  </si>
+  <si>
+    <t>SKIPPED INITIALLY</t>
+  </si>
+  <si>
+    <t>$t2 = 0xBFC00000</t>
+  </si>
+  <si>
+    <t>$t2 = 0xBFC00020</t>
+  </si>
+  <si>
+    <t>0x0000</t>
+  </si>
+  <si>
+    <t>0x0004</t>
+  </si>
+  <si>
+    <t>0x0008</t>
+  </si>
+  <si>
+    <t>0x001C</t>
+  </si>
+  <si>
+    <t>0x000C</t>
+  </si>
+  <si>
+    <t>0x0010</t>
+  </si>
+  <si>
+    <t>0x0014</t>
+  </si>
+  <si>
+    <t>0x0018</t>
+  </si>
+  <si>
+    <t>0x0020</t>
+  </si>
+  <si>
+    <t>0x0024</t>
+  </si>
+  <si>
+    <t>0x0028</t>
+  </si>
+  <si>
+    <t>0x002C</t>
+  </si>
+  <si>
+    <t>0x0030</t>
+  </si>
+  <si>
+    <t>0x0034</t>
+  </si>
+  <si>
+    <t>0x0038</t>
+  </si>
+  <si>
+    <t>0x003C</t>
+  </si>
+  <si>
+    <t>0x0040</t>
+  </si>
+  <si>
+    <t>JUMP to 0x0014</t>
+  </si>
+  <si>
+    <t>JUMP to 0x0028</t>
+  </si>
+  <si>
+    <t>JUMP to 0x0020</t>
+  </si>
+  <si>
+    <t>$v0 = 0xFFFF0000</t>
+  </si>
+  <si>
+    <t>STP</t>
+  </si>
+  <si>
+    <t>$v0 = 0x0000003C</t>
+  </si>
+  <si>
+    <t>$ra = 0x0000002C</t>
+  </si>
+  <si>
+    <t>JUMP to 0x0000</t>
+  </si>
+  <si>
+    <t>TEST ALL ALU INSTRUCTIONS</t>
+  </si>
+  <si>
+    <t>TEST ALL JUMPS</t>
+  </si>
+  <si>
+    <t>$t1 = 0x00000001</t>
+  </si>
+  <si>
+    <t>$t2 = 0x00000010</t>
+  </si>
+  <si>
+    <t>$s1 = 0xFFFFFFFF</t>
+  </si>
+  <si>
+    <t>Branch does not happen</t>
+  </si>
+  <si>
+    <t>Branch happens</t>
+  </si>
+  <si>
+    <t>$s2 = 0xFFFFFFFE</t>
+  </si>
+  <si>
+    <t>$s1 = 0xFFFF0000</t>
+  </si>
+  <si>
+    <t>$v0 = 0x00000002</t>
+  </si>
+  <si>
+    <t>$v0 = 0x00000003</t>
+  </si>
+  <si>
+    <t>$ra = 0x00000048</t>
+  </si>
+  <si>
+    <t>mem[256] = 0x00000048</t>
+  </si>
+  <si>
+    <t>$v0 = 0x00000005</t>
+  </si>
+  <si>
+    <t>$v0 = 0x00000006</t>
+  </si>
+  <si>
+    <t>$v0 = 0x00000007</t>
+  </si>
+  <si>
+    <t>$ra = 0x00000108</t>
+  </si>
+  <si>
+    <t>mem[257] = 0x00000108</t>
+  </si>
+  <si>
+    <t>$v0 = 0x00000008</t>
+  </si>
+  <si>
+    <t>TESTS ALL BRANCHES</t>
+  </si>
+  <si>
+    <t>$t2 = 0x00000007</t>
+  </si>
+  <si>
+    <t>HI = 0xFFFFFFFF</t>
+  </si>
+  <si>
+    <t>LO = 0xFFFFFFF9</t>
+  </si>
+  <si>
+    <t>$v0 = 0xFFFFFFFF</t>
+  </si>
+  <si>
+    <t>$v0 = 0xFFFFFFF9</t>
+  </si>
+  <si>
+    <t>HI = 0x00000000</t>
+  </si>
+  <si>
+    <t>LO = 0x0006fff9</t>
+  </si>
+  <si>
+    <t>$v0 = 0x0006FFF9</t>
+  </si>
+  <si>
+    <t>$t1 = 0x88880000</t>
+  </si>
+  <si>
+    <t>$t1 = 0x8888888B</t>
+  </si>
+  <si>
+    <t>$t2 = 0x44440000</t>
+  </si>
+  <si>
+    <t>$t2 = 0x44444444</t>
+  </si>
+  <si>
+    <t>HI = 0x00000003</t>
+  </si>
+  <si>
+    <t>LO = 0x00000002</t>
+  </si>
+  <si>
+    <t>$t0 = 0xFFFF0000</t>
+  </si>
+  <si>
+    <t>HI = 0xFFFF0000</t>
+  </si>
+  <si>
+    <t>$v0 = 0xFFFF00000</t>
+  </si>
+  <si>
+    <t>$t0 = 0xFFFF1111</t>
+  </si>
+  <si>
+    <t>LO = 0xFFFF1111</t>
+  </si>
+  <si>
+    <t>$v0 = 0xFFFF1111</t>
+  </si>
+  <si>
+    <t>TESTS ALL MOVES</t>
+  </si>
+  <si>
+    <t>$t1 = 0x8888888E</t>
+  </si>
+  <si>
+    <t>HI = 0x00000006</t>
+  </si>
+  <si>
+    <t>LO = 0x(3)C0000002</t>
+  </si>
+  <si>
+    <t>$v0 = 0xC0000002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +439,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -229,10 +483,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,96 +1049,96 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD59C4A-B29B-4ADE-81FA-F6E846077368}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A26"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="1" max="1" width="24.6328125" customWidth="1"/>
     <col min="2" max="2" width="18.453125" customWidth="1"/>
     <col min="3" max="3" width="15.54296875" customWidth="1"/>
     <col min="4" max="4" width="16.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -920,8 +1178,14 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -936,12 +1200,710 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E61ED3-9DDA-478F-8659-D8592208CEDF}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="16.36328125" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6943B04D-2065-4FEA-A20C-379324EDF794}">
+  <dimension ref="A1:H56"/>
+  <sheetViews>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" customWidth="1"/>
+    <col min="4" max="4" width="15.08984375" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" customWidth="1"/>
+    <col min="7" max="7" width="20.81640625" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="3"/>
+      <c r="F5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4286F6-7198-49D1-A25F-2C5BE24259E5}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DEEFFCF-2652-4491-A5AF-8712E7E94359}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" activeCellId="1" sqref="D24 C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.36328125" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="18.36328125" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>